<commit_message>
Fix OLS index error, add classification and ROC curve
</commit_message>
<xml_diff>
--- a/results/figures/Axial_model_summary.xlsx
+++ b/results/figures/Axial_model_summary.xlsx
@@ -481,11 +481,21 @@
           <t>0-3 mo.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15.999</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="F2" t="n">
+        <v>234.35</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,11 +508,21 @@
           <t>3-6 mo.</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>-1.451</v>
+      </c>
+      <c r="D3" t="n">
+        <v>33.237</v>
+      </c>
+      <c r="E3" t="n">
+        <v>26.695</v>
+      </c>
+      <c r="F3" t="n">
+        <v>232.136</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -515,11 +535,21 @@
           <t>6-12 mo.</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>-1.336</v>
+      </c>
+      <c r="D4" t="n">
+        <v>38.425</v>
+      </c>
+      <c r="E4" t="n">
+        <v>30.355</v>
+      </c>
+      <c r="F4" t="n">
+        <v>238.328</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -532,11 +562,21 @@
           <t>0-3 mo.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="D5" t="n">
+        <v>17.608</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.866</v>
+      </c>
+      <c r="F5" t="n">
+        <v>236.27</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -549,11 +589,21 @@
           <t>3-6 mo.</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>-1.519</v>
+      </c>
+      <c r="D6" t="n">
+        <v>33.697</v>
+      </c>
+      <c r="E6" t="n">
+        <v>26.396</v>
+      </c>
+      <c r="F6" t="n">
+        <v>232.805</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -566,11 +616,21 @@
           <t>6-12 mo.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>-1.404</v>
+      </c>
+      <c r="D7" t="n">
+        <v>38.973</v>
+      </c>
+      <c r="E7" t="n">
+        <v>30.127</v>
+      </c>
+      <c r="F7" t="n">
+        <v>240.285</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -587,9 +647,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -606,9 +664,7 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -625,9 +681,7 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>